<commit_message>
Corrección de issue #14
</commit_message>
<xml_diff>
--- a/CasosUso/Casos de uso.xlsx
+++ b/CasosUso/Casos de uso.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CU_01" sheetId="5" r:id="rId1"/>
@@ -190,33 +195,6 @@
 eliminar el regrsitro del material seleccionado</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Abre la ventana </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>agregar materiales</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> en modo de solo vista,
-con la informacion del proveedor seleccionado</t>
-    </r>
-  </si>
-  <si>
     <t>Genera un archivo de excel con la  lsita de materiales
 y la guarda en la computadora</t>
   </si>
@@ -592,33 +570,6 @@
   </si>
   <si>
     <t>Nombre ventana: Inicio de sesión</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Abre la ventana </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>agregar materiales</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> en modo de edicion,
-con la informacion del material seleccionado.</t>
-    </r>
   </si>
   <si>
     <t>Abre la ventana sesión en modo de edición,
@@ -709,12 +660,20 @@
 Actualiza la tabla de sesiones
 </t>
   </si>
+  <si>
+    <t>Abre la ventana agregar materiales en modo de solo vista,
+con la informacion del proveedor seleccionado</t>
+  </si>
+  <si>
+    <t>Abre la ventana agregar materiales en modo de edicion,
+con la informacion del material seleccionado.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1259,6 +1218,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1274,9 +1263,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1304,39 +1290,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1349,15 +1335,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1386,24 +1363,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1537,7 +1496,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1581,7 +1540,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1630,7 +1589,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1674,7 +1633,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1717,7 +1676,7 @@
         <xdr:cNvPr id="8" name="Imagen 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A13C58F-FF3E-4363-9C21-FB49734F92ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A13C58F-FF3E-4363-9C21-FB49734F92ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1789,7 +1748,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1821,9 +1780,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1855,6 +1815,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2030,14 +1991,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -2047,73 +2008,73 @@
     <col min="6" max="6" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1">
+      <c r="D1" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="B2" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-    </row>
-    <row r="4" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="5" spans="1:9">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-    </row>
-    <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="8" spans="1:9">
+      <c r="B6" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>6</v>
       </c>
@@ -2123,52 +2084,52 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="C10" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1">
+      <c r="C11" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>12</v>
       </c>
@@ -2178,68 +2139,68 @@
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
-    </row>
-    <row r="15" spans="1:9" ht="52.5" customHeight="1">
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="52"/>
+    </row>
+    <row r="15" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:9" ht="69.75" customHeight="1">
+      <c r="B15" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="B16" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-    </row>
-    <row r="18" spans="1:6" ht="90.75" customHeight="1">
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+    </row>
+    <row r="18" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="63" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6">
+      <c r="B18" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>14</v>
       </c>
@@ -2249,15 +2210,15 @@
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="64"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66"/>
-    </row>
-    <row r="22" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="45"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="48"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -2265,7 +2226,7 @@
       <c r="E22" s="48"/>
       <c r="F22" s="48"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>15</v>
       </c>
@@ -2275,89 +2236,89 @@
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A24" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="44"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="46"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="47"/>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="57"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="47"/>
+      <c r="F26" s="58"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
       <c r="D27" s="48"/>
       <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="47"/>
+      <c r="F27" s="58"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="57"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
       <c r="D28" s="48"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="49"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="47"/>
+      <c r="F28" s="58"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="47"/>
+      <c r="F29" s="58"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
       <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="47"/>
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="57"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
-      <c r="F31" s="49"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="47"/>
+      <c r="F31" s="58"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="57"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
       <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
-    </row>
-    <row r="33" spans="1:6" ht="121.5" customHeight="1" thickBot="1">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="52"/>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="F32" s="58"/>
+    </row>
+    <row r="33" spans="1:6" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="59"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>16</v>
       </c>
@@ -2377,7 +2338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>33</v>
       </c>
@@ -2394,10 +2355,10 @@
         <v>37</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>34</v>
       </c>
@@ -2414,55 +2375,54 @@
         <v>37</v>
       </c>
       <c r="F36" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A37" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="53" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="42"/>
       <c r="D38" s="42"/>
       <c r="E38" s="42"/>
-      <c r="F38" s="54"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A39" s="55"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
+      <c r="F38" s="63"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="64"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F33"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:F39"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
@@ -2475,11 +2435,12 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F33"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2487,14 +2448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -2504,7 +2465,7 @@
     <col min="6" max="6" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2514,63 +2475,63 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1">
+      <c r="D1" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="B2" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-    </row>
-    <row r="4" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="5" spans="1:9">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1">
+      <c r="B5" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-    </row>
-    <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="8" spans="1:9">
+      <c r="B6" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>6</v>
       </c>
@@ -2580,52 +2541,52 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="C10" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1">
+      <c r="C11" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>12</v>
       </c>
@@ -2635,44 +2596,44 @@
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
-    </row>
-    <row r="15" spans="1:9" ht="52.5" customHeight="1">
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="52"/>
+    </row>
+    <row r="15" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:9" ht="69.75" customHeight="1">
+      <c r="B15" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="18" spans="1:6">
+      <c r="B16" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>14</v>
       </c>
@@ -2682,15 +2643,15 @@
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="64"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
-    </row>
-    <row r="20" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="48"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
@@ -2698,7 +2659,7 @@
       <c r="E20" s="48"/>
       <c r="F20" s="48"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>15</v>
       </c>
@@ -2708,89 +2669,89 @@
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A22" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="44"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="47"/>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="54"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="56"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="47"/>
+      <c r="F24" s="58"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="57"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
       <c r="D25" s="48"/>
       <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="47"/>
+      <c r="F25" s="58"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="57"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="47"/>
+      <c r="F26" s="58"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
       <c r="D27" s="48"/>
       <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="47"/>
+      <c r="F27" s="58"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="57"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
       <c r="D28" s="48"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="49"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="47"/>
+      <c r="F28" s="58"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="47"/>
+      <c r="F29" s="58"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
       <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
-    </row>
-    <row r="31" spans="1:6" ht="121.5" customHeight="1" thickBot="1">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="52"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="1:6" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="59"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="61"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>16</v>
       </c>
@@ -2810,30 +2771,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" customHeight="1">
-      <c r="A34" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="B34" s="18" t="s">
         <v>25</v>
       </c>
@@ -2847,35 +2808,34 @@
         <v>25</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="42"/>
       <c r="D35" s="42"/>
       <c r="E35" s="42"/>
-      <c r="F35" s="54"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A36" s="55"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="57"/>
+      <c r="F35" s="63"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="64"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F31"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A20:F20"/>
@@ -2886,11 +2846,12 @@
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F31"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2899,14 +2860,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -2916,7 +2877,7 @@
     <col min="6" max="6" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2926,63 +2887,63 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1">
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-    </row>
-    <row r="4" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="5" spans="1:9">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1">
+      <c r="B5" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-    </row>
-    <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="8" spans="1:9">
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>6</v>
       </c>
@@ -2992,108 +2953,108 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1">
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>12</v>
       </c>
@@ -3103,56 +3064,56 @@
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
-    </row>
-    <row r="19" spans="1:6" ht="52.5" customHeight="1">
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="52"/>
+    </row>
+    <row r="19" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+    </row>
+    <row r="20" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-    </row>
-    <row r="20" spans="1:6" ht="69.75" customHeight="1">
-      <c r="A20" s="10" t="s">
+      <c r="B20" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6">
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>14</v>
       </c>
@@ -3162,15 +3123,15 @@
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="64"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66"/>
-    </row>
-    <row r="25" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="48"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
@@ -3178,7 +3139,7 @@
       <c r="E25" s="48"/>
       <c r="F25" s="48"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>15</v>
       </c>
@@ -3188,89 +3149,89 @@
       <c r="E26" s="42"/>
       <c r="F26" s="42"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A27" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="44"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="47"/>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="47"/>
+      <c r="F29" s="58"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
       <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="47"/>
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="57"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
-      <c r="F31" s="49"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="47"/>
+      <c r="F31" s="58"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="57"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
       <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="47"/>
+      <c r="F32" s="58"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="57"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
-      <c r="F33" s="49"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="47"/>
+      <c r="F33" s="58"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="57"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
       <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="47"/>
+      <c r="F34" s="58"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="57"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
       <c r="D35" s="48"/>
       <c r="E35" s="48"/>
-      <c r="F35" s="49"/>
-    </row>
-    <row r="36" spans="1:8" ht="121.5" customHeight="1" thickBot="1">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52"/>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="F35" s="58"/>
+    </row>
+    <row r="36" spans="1:8" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="61"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -3291,9 +3252,9 @@
       </c>
       <c r="H37" s="26"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>25</v>
@@ -3308,10 +3269,10 @@
         <v>25</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
@@ -3331,7 +3292,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>50</v>
       </c>
@@ -3348,10 +3309,10 @@
         <v>25</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="42.75" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>51</v>
       </c>
@@ -3368,10 +3329,10 @@
         <v>25</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="35.25" customHeight="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>24</v>
       </c>
@@ -3391,7 +3352,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="48" customHeight="1">
+    <row r="43" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>52</v>
       </c>
@@ -3408,48 +3369,48 @@
         <v>25</v>
       </c>
       <c r="F43" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="30">
-      <c r="A44" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="53" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
       <c r="E45" s="42"/>
-      <c r="F45" s="54"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A46" s="55"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="57"/>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="F45" s="63"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="64"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="66"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="42" t="s">
         <v>15</v>
       </c>
@@ -3459,89 +3420,89 @@
       <c r="E47" s="42"/>
       <c r="F47" s="42"/>
     </row>
-    <row r="48" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A48" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="44"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="46"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="47"/>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="56"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="57"/>
       <c r="B50" s="48"/>
       <c r="C50" s="48"/>
       <c r="D50" s="48"/>
       <c r="E50" s="48"/>
-      <c r="F50" s="49"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="47"/>
+      <c r="F50" s="58"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="57"/>
       <c r="B51" s="48"/>
       <c r="C51" s="48"/>
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="47"/>
+      <c r="F51" s="58"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="57"/>
       <c r="B52" s="48"/>
       <c r="C52" s="48"/>
       <c r="D52" s="48"/>
       <c r="E52" s="48"/>
-      <c r="F52" s="49"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="47"/>
+      <c r="F52" s="58"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="57"/>
       <c r="B53" s="48"/>
       <c r="C53" s="48"/>
       <c r="D53" s="48"/>
       <c r="E53" s="48"/>
-      <c r="F53" s="49"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="47"/>
+      <c r="F53" s="58"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="57"/>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
       <c r="D54" s="48"/>
       <c r="E54" s="48"/>
-      <c r="F54" s="49"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="47"/>
+      <c r="F54" s="58"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="57"/>
       <c r="B55" s="48"/>
       <c r="C55" s="48"/>
       <c r="D55" s="48"/>
       <c r="E55" s="48"/>
-      <c r="F55" s="49"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="47"/>
+      <c r="F55" s="58"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="57"/>
       <c r="B56" s="48"/>
       <c r="C56" s="48"/>
       <c r="D56" s="48"/>
       <c r="E56" s="48"/>
-      <c r="F56" s="49"/>
-    </row>
-    <row r="57" spans="1:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="A57" s="50"/>
-      <c r="B57" s="51"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="52"/>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="F56" s="58"/>
+    </row>
+    <row r="57" spans="1:6" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="59"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="61"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>16</v>
       </c>
@@ -3561,29 +3522,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="22" t="s">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>26</v>
@@ -3592,18 +3553,18 @@
         <v>20</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F60" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>26</v>
@@ -3612,38 +3573,38 @@
         <v>30</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F61" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="11" t="s">
+      <c r="B62" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>66</v>
       </c>
       <c r="C62" s="18">
         <v>10</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F62" s="22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="25.5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>26</v>
@@ -3652,18 +3613,18 @@
         <v>50</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="30">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>26</v>
@@ -3672,39 +3633,39 @@
         <v>50</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E64" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F64" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="18" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="C65" s="18">
         <v>10</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E65" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F65" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="57.75" customHeight="1">
-      <c r="A66" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="B66" s="18" t="s">
         <v>25</v>
       </c>
@@ -3718,35 +3679,45 @@
         <v>25</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="42"/>
       <c r="D67" s="42"/>
       <c r="E67" s="42"/>
-      <c r="F67" s="54"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A68" s="55"/>
-      <c r="B68" s="56"/>
-      <c r="C68" s="56"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="56"/>
-      <c r="F68" s="57"/>
+      <c r="F67" s="63"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="64"/>
+      <c r="B68" s="65"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="65"/>
+      <c r="F68" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:F57"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F36"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C15:F15"/>
@@ -3756,22 +3727,12 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F36"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A49:F57"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3780,14 +3741,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
@@ -3797,73 +3758,73 @@
     <col min="6" max="6" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="64" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1">
+      <c r="D1" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="B2" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-    </row>
-    <row r="4" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="5" spans="1:9">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1">
+      <c r="B5" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-    </row>
-    <row r="7" spans="1:9" ht="5.25" customHeight="1"/>
-    <row r="8" spans="1:9">
+      <c r="B6" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>6</v>
       </c>
@@ -3873,108 +3834,108 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="C9" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="C10" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="C11" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="C12" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="59" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="C13" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-    </row>
-    <row r="15" spans="1:9" ht="33" customHeight="1">
+      <c r="C14" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1">
+      <c r="C15" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>12</v>
       </c>
@@ -3984,56 +3945,56 @@
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
-    </row>
-    <row r="19" spans="1:6" ht="52.5" customHeight="1">
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="52"/>
+    </row>
+    <row r="19" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+    </row>
+    <row r="20" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="63" t="s">
-        <v>187</v>
-      </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-    </row>
-    <row r="20" spans="1:6" ht="69.75" customHeight="1">
-      <c r="A20" s="10" t="s">
+      <c r="B20" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6">
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>14</v>
       </c>
@@ -4043,15 +4004,15 @@
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="64"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66"/>
-    </row>
-    <row r="25" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="48"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
@@ -4059,7 +4020,7 @@
       <c r="E25" s="48"/>
       <c r="F25" s="48"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>15</v>
       </c>
@@ -4069,89 +4030,89 @@
       <c r="E26" s="42"/>
       <c r="F26" s="42"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A27" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="44"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="47"/>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="47"/>
+      <c r="F29" s="58"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
       <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="47"/>
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="57"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
-      <c r="F31" s="49"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="47"/>
+      <c r="F31" s="58"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="57"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
       <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="47"/>
+      <c r="F32" s="58"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="57"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
-      <c r="F33" s="49"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="47"/>
+      <c r="F33" s="58"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="57"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
       <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="47"/>
+      <c r="F34" s="58"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="57"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
       <c r="D35" s="48"/>
       <c r="E35" s="48"/>
-      <c r="F35" s="49"/>
-    </row>
-    <row r="36" spans="1:6" ht="121.5" customHeight="1" thickBot="1">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="F35" s="58"/>
+    </row>
+    <row r="36" spans="1:6" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="61"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -4171,9 +4132,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>25</v>
@@ -4188,10 +4149,10 @@
         <v>25</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
@@ -4208,108 +4169,108 @@
         <v>25</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A41" s="11" t="s">
+      <c r="B41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="15" t="s">
+      <c r="B42" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="21" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A42" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A43" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="21" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="53" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="42"/>
       <c r="D44" s="42"/>
       <c r="E44" s="42"/>
-      <c r="F44" s="54"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A45" s="55"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="57"/>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="F44" s="63"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="64"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="66"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="42" t="s">
         <v>15</v>
       </c>
@@ -4319,89 +4280,89 @@
       <c r="E46" s="42"/>
       <c r="F46" s="42"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A47" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="44"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="46"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="47"/>
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="56"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="57"/>
       <c r="B49" s="48"/>
       <c r="C49" s="48"/>
       <c r="D49" s="48"/>
       <c r="E49" s="48"/>
-      <c r="F49" s="49"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="47"/>
+      <c r="F49" s="58"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="57"/>
       <c r="B50" s="48"/>
       <c r="C50" s="48"/>
       <c r="D50" s="48"/>
       <c r="E50" s="48"/>
-      <c r="F50" s="49"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="47"/>
+      <c r="F50" s="58"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="57"/>
       <c r="B51" s="48"/>
       <c r="C51" s="48"/>
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="47"/>
+      <c r="F51" s="58"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="57"/>
       <c r="B52" s="48"/>
       <c r="C52" s="48"/>
       <c r="D52" s="48"/>
       <c r="E52" s="48"/>
-      <c r="F52" s="49"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="47"/>
+      <c r="F52" s="58"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="57"/>
       <c r="B53" s="48"/>
       <c r="C53" s="48"/>
       <c r="D53" s="48"/>
       <c r="E53" s="48"/>
-      <c r="F53" s="49"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="47"/>
+      <c r="F53" s="58"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="57"/>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
       <c r="D54" s="48"/>
       <c r="E54" s="48"/>
-      <c r="F54" s="49"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="47"/>
+      <c r="F54" s="58"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="57"/>
       <c r="B55" s="48"/>
       <c r="C55" s="48"/>
       <c r="D55" s="48"/>
       <c r="E55" s="48"/>
-      <c r="F55" s="49"/>
-    </row>
-    <row r="56" spans="1:6" ht="87.75" customHeight="1" thickBot="1">
-      <c r="A56" s="50"/>
-      <c r="B56" s="51"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="52"/>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="F55" s="58"/>
+    </row>
+    <row r="56" spans="1:6" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="59"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="61"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>16</v>
       </c>
@@ -4421,9 +4382,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>25</v>
@@ -4438,12 +4399,12 @@
         <v>25</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="30">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>26</v>
@@ -4452,18 +4413,18 @@
         <v>20</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F59" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>26</v>
@@ -4472,38 +4433,38 @@
         <v>30</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F60" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C61" s="18">
         <v>10</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="30" customHeight="1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>26</v>
@@ -4512,38 +4473,38 @@
         <v>50</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="18">
         <v>10</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>26</v>
@@ -4552,18 +4513,18 @@
         <v>100</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="66" customHeight="1">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>25</v>
@@ -4578,35 +4539,42 @@
         <v>25</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="53" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="62" t="s">
         <v>22</v>
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="42"/>
       <c r="D66" s="42"/>
       <c r="E66" s="42"/>
-      <c r="F66" s="54"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A67" s="55"/>
-      <c r="B67" s="56"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="57"/>
+      <c r="F66" s="63"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="64"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="65"/>
+      <c r="F67" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A28:F36"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F56"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
@@ -4619,19 +4587,12 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A28:F36"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F56"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4640,14 +4601,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -4657,47 +4618,47 @@
     <col min="6" max="6" width="48.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="73" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="75"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="D1" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="69"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="90" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="86" t="s">
-        <v>140</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="B3" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -4705,31 +4666,31 @@
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="86" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="B5" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="B6" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
@@ -4737,115 +4698,115 @@
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="68" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="91"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>1</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="86" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="C10" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>2</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="67" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>3</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="C12" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <v>4</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="86" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-    </row>
-    <row r="14" spans="1:6">
+        <v>143</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>5</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="C14" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>6</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="86" t="s">
-        <v>149</v>
-      </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-    </row>
-    <row r="16" spans="1:6">
+        <v>143</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
@@ -4853,53 +4814,53 @@
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="68" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="89"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="76"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>6</v>
       </c>
-      <c r="B19" s="90" t="s">
-        <v>150</v>
-      </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="B19" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="86" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="B20" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
@@ -4907,125 +4868,125 @@
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="68" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="73"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="75"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="76"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="68" t="s">
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="68"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="82"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="78"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="80"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="81"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="82"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="81"/>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="82"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="81"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="82"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="81"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="82"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="81"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="82"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="81"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="82"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="81"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="82"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A35" s="83"/>
-      <c r="B35" s="84"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="85"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="83" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="84"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="86"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="87"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="88"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="87"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="88"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="87"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="88"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="87"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="88"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="87"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="88"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="87"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="88"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="87"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="88"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="89"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="91"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
         <v>16</v>
       </c>
@@ -5045,133 +5006,133 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="C37" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>155</v>
       </c>
       <c r="D37" s="40"/>
       <c r="E37" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="41" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="38" t="s">
-        <v>158</v>
-      </c>
       <c r="B38" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>155</v>
       </c>
       <c r="D38" s="39"/>
       <c r="E38" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="38" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="38" t="s">
-        <v>160</v>
-      </c>
       <c r="B39" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>155</v>
       </c>
       <c r="D39" s="39"/>
       <c r="E39" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" s="41" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="38" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="38" t="s">
-        <v>162</v>
-      </c>
       <c r="B40" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>155</v>
       </c>
       <c r="D40" s="39"/>
       <c r="E40" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F40" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="38" t="s">
         <v>48</v>
       </c>
       <c r="B41" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>155</v>
       </c>
       <c r="D41" s="39"/>
       <c r="E41" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="F41" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="F41" s="41" t="s">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="38" t="s">
-        <v>166</v>
-      </c>
       <c r="B42" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>155</v>
       </c>
       <c r="D42" s="39"/>
       <c r="E42" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="67" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="69"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A44" s="70"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="72"/>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="78"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="79"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="81"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="31"/>
       <c r="C45" s="31"/>
@@ -5181,6 +5142,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F35"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B2:F2"/>
@@ -5193,19 +5167,6 @@
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>